<commit_message>
changes to final project, not everything is working yet
</commit_message>
<xml_diff>
--- a/11-Final-Project/tasks.xlsx
+++ b/11-Final-Project/tasks.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c43810eba78802c5/spiced/random-forest-fennel-student-code/11-Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="8_{767E4AAB-8E10-9A4F-B39F-FAC51C8A202B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E49ACFA-6FCC-3740-A250-D2005AA4E9CA}"/>
+  <xr:revisionPtr revIDLastSave="506" documentId="8_{767E4AAB-8E10-9A4F-B39F-FAC51C8A202B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE34BB77-85F3-2840-A9F7-3B9EA3E908C1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" activeTab="1" xr2:uid="{C712685F-EEBF-B146-924B-85EB1F1EB693}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" activeTab="3" xr2:uid="{C712685F-EEBF-B146-924B-85EB1F1EB693}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Parts" sheetId="2" r:id="rId1"/>
     <sheet name="Project Plan" sheetId="1" r:id="rId2"/>
     <sheet name="Web App" sheetId="3" r:id="rId3"/>
+    <sheet name="Ideas" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Project Plan'!$A$3:$D$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Project Plan'!$A$3:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
   <si>
     <t>Complete by</t>
   </si>
@@ -194,9 +195,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>To Start</t>
-  </si>
-  <si>
     <t>Task Name</t>
   </si>
   <si>
@@ -251,9 +249,6 @@
     <t>Refactor code with pylint</t>
   </si>
   <si>
-    <t>Return full dataset for particular company</t>
-  </si>
-  <si>
     <t>Docker/Heroku</t>
   </si>
   <si>
@@ -273,6 +268,15 @@
   </si>
   <si>
     <t>Add on conflict update sentiment score</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Return full dataset for search keyword</t>
+  </si>
+  <si>
+    <t>Make ETL repeat itself once it's done</t>
   </si>
 </sst>
 </file>
@@ -717,320 +721,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4131BA-65FA-F04F-BCEA-17358AB8997C}">
-  <dimension ref="A2:Q16"/>
+  <dimension ref="A2:M16"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="17" max="17" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="8" t="s">
         <v>49</v>
       </c>
+      <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
-        <v>5</v>
+      <c r="F2" s="4"/>
+      <c r="G2" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="I2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="14" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="16" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="M3" s="13" t="s">
+      <c r="K3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="15"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="15"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="Q4" s="15"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="Q5" s="15"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G5" s="11"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G6" s="11"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="D7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="Q7" s="15"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G7" s="11"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="Q8" s="15"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G8" s="11"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="Q9" s="15"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G9" s="11"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="Q10" s="15"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G10" s="11"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="Q11" s="15"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G11" s="11"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="Q12" s="15"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G12" s="11"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="Q13" s="15"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G13" s="11"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="Q14" s="15"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="Q15" s="15"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G15" s="11"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="Q16" s="15"/>
+      <c r="G16" s="11"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="M16" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1039,10 +957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C651200-C242-2F4B-B27E-572AFB8F5B56}">
-  <dimension ref="A2:N27"/>
+  <dimension ref="A2:N26"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,7 +974,7 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H2" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>49</v>
@@ -1065,21 +983,21 @@
         <v>2</v>
       </c>
       <c r="K2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>63</v>
-      </c>
       <c r="M2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>47</v>
@@ -1134,31 +1052,31 @@
         <v>6</v>
       </c>
       <c r="H4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,H$3)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,H$3)</f>
         <v>1</v>
       </c>
       <c r="I4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,I3)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,I3)</f>
         <v>10.5</v>
       </c>
       <c r="J4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,J3)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,J3)</f>
+        <v>5.5</v>
+      </c>
+      <c r="K4" s="17">
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,K3)</f>
+        <v>5</v>
+      </c>
+      <c r="L4" s="17">
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,L3)</f>
+        <v>13</v>
+      </c>
+      <c r="M4" s="17">
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,M3)</f>
         <v>6</v>
       </c>
-      <c r="K4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,K3)</f>
-        <v>5</v>
-      </c>
-      <c r="L4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,L3)</f>
-        <v>13</v>
-      </c>
-      <c r="M4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,M3)</f>
-        <v>6</v>
-      </c>
       <c r="N4" s="17">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,N3)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,N3)</f>
         <v>0</v>
       </c>
     </row>
@@ -1182,31 +1100,31 @@
         <v>6</v>
       </c>
       <c r="H5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,H$3,$E$4:$E$103,$G5)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,H$3,$E$4:$E$102,$G5)</f>
         <v>1</v>
       </c>
       <c r="I5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,I$3,$E$4:$E$103,$G5)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,I$3,$E$4:$E$102,$G5)</f>
         <v>10.5</v>
       </c>
       <c r="J5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,J$3,$E$4:$E$103,$G5)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,J$3,$E$4:$E$102,$G5)</f>
+        <v>4</v>
+      </c>
+      <c r="K5" s="21">
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,K$3,$E$4:$E$102,$G5)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,K$3,$E$4:$E$103,$G5)</f>
+      <c r="L5" s="21">
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,L$3,$E$4:$E$102,$G5)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,L$3,$E$4:$E$103,$G5)</f>
+      <c r="M5" s="21">
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,M$3,$E$4:$E$102,$G5)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,M$3,$E$4:$E$103,$G5)</f>
-        <v>0</v>
-      </c>
       <c r="N5" s="21">
-        <f>SUMIFS($C$4:$C$103,$D$4:$D$103,N$3,$E$4:$E$103,$G5)</f>
+        <f>SUMIFS($C$4:$C$102,$D$4:$D$102,N$3,$E$4:$E$102,$G5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1227,7 +1145,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H6" s="20">
         <f>H4-H5</f>
@@ -1239,7 +1157,7 @@
       </c>
       <c r="J6" s="20">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="K6" s="20">
         <f t="shared" si="0"/>
@@ -1260,7 +1178,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -1277,7 +1195,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -1294,7 +1212,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -1311,7 +1229,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>49</v>
@@ -1328,7 +1246,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -1379,66 +1297,75 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
       </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
       </c>
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
       </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1449,13 +1376,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
@@ -1463,16 +1390,16 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1497,7 +1424,7 @@
         <v>49</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -1505,13 +1432,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>37</v>
@@ -1519,16 +1446,16 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1536,7 +1463,7 @@
         <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1550,26 +1477,12 @@
         <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1583,7 +1496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81ECF023-597C-0142-BED1-D5887D540AB6}">
   <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1605,7 +1520,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1646,7 +1561,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D800561-A125-E642-8D3C-EF3836778EDE}">
+  <dimension ref="B3:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>